<commit_message>
Checks for dates, if dates have big difference it will create another sheet declaring as a 2nd session.
</commit_message>
<xml_diff>
--- a/original_files/ACCT.xlsx
+++ b/original_files/ACCT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\PycharmProjects\xceltest\original_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\PycharmProjects\uniScheduler\original_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919A500F-49D7-48E8-BE16-7AA4146E04C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22573BD-333E-419C-A8A7-3BFA609C7700}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,8 +825,12 @@
         <v>24</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="K4" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L4" s="2">
+        <v>43756</v>
+      </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -848,8 +852,12 @@
       <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="K5" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L5" s="2">
+        <v>43812</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -870,8 +878,12 @@
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L6" s="2">
+        <v>43756</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -892,6 +904,12 @@
       <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="K7" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L7" s="2">
+        <v>43812</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -912,6 +930,12 @@
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K8" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L8" s="2">
+        <v>43756</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -932,6 +956,12 @@
       <c r="H9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="K9" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L9" s="2">
+        <v>43812</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -972,6 +1002,12 @@
       <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="K11" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L11" s="2">
+        <v>43756</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -991,6 +1027,12 @@
       </c>
       <c r="H12" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="K12" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L12" s="2">
+        <v>43812</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1083,8 +1125,12 @@
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="K16" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L16" s="2">
+        <v>43756</v>
+      </c>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1105,6 +1151,12 @@
       </c>
       <c r="H17" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="K17" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L17" s="2">
+        <v>43812</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1173,6 +1225,12 @@
       <c r="H20" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="K20" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L20" s="2">
+        <v>43756</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1193,6 +1251,12 @@
       <c r="H21" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="K21" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L21" s="2">
+        <v>43812</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1293,6 +1357,12 @@
       <c r="H26" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="K26" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L26" s="2">
+        <v>43756</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1313,6 +1383,12 @@
       <c r="H27" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K27" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L27" s="2">
+        <v>43812</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -1414,7 +1490,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>22</v>
       </c>
@@ -1425,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>22</v>
       </c>
@@ -1445,7 +1521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>22</v>
       </c>
@@ -1464,8 +1540,14 @@
       <c r="H35" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K35" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L35" s="2">
+        <v>43756</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>22</v>
       </c>
@@ -1484,8 +1566,14 @@
       <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K36" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L36" s="2">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>22</v>
       </c>
@@ -1504,8 +1592,14 @@
       <c r="H37" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K37" s="2">
+        <v>43702</v>
+      </c>
+      <c r="L37" s="2">
+        <v>43756</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>22</v>
       </c>
@@ -1524,8 +1618,14 @@
       <c r="H38" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K38" s="2">
+        <v>43759</v>
+      </c>
+      <c r="L38" s="2">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>22</v>
       </c>
@@ -1545,7 +1645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H41" s="8"/>
     </row>
     <row r="55" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>